<commit_message>
docs/cosmos_vcore.md re: config and link
</commit_message>
<xml_diff>
--- a/data/search_results/compared_results.xlsx
+++ b/data/search_results/compared_results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chjoakim\github\azure-cosmos-db-vector-search-openai-python\data\search_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F028ACD-AEE1-4E20-B28E-43227C726689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C5E529-7727-413D-9349-73B40A4C448C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="3120" windowWidth="30950" windowHeight="17090"/>
+    <workbookView xWindow="3630" yWindow="3900" windowWidth="30950" windowHeight="17090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="compared_results" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1135,11 +1135,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2210,4 +2211,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>